<commit_message>
Added delete_empty_rows and delete_past_homework functions
</commit_message>
<xml_diff>
--- a/DiscordExcel.xlsx
+++ b/DiscordExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Zhang\PycharmProjects\webscraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliss\PycharmProjects\Hackulator_HomeworkBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FA597-80CE-46E5-9B8E-2A52095F72E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1F2BAC-6B35-4753-917D-84A559A538A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20E8DD84-1E46-4477-AFF1-EA600C6169F9}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18500" windowHeight="10510" xr2:uid="{20E8DD84-1E46-4477-AFF1-EA600C6169F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,22 +458,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AFA9C-7080-4BCB-B2DE-D0171F1DAEC9}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -507,7 +507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -524,24 +524,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>1537</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -549,46 +535,63 @@
         <v>1537</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>1113</v>
+        <v>1537</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>1113</v>
       </c>
       <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1113</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>